<commit_message>
Fixed CSS allowing image placement; more functions
</commit_message>
<xml_diff>
--- a/documentation/infant-sleep_action_behaviors.xlsx
+++ b/documentation/infant-sleep_action_behaviors.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -153,12 +153,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color theme="0" tint="-0.34998626667073579"/>
@@ -443,7 +438,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +544,7 @@
     <mergeCell ref="B1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Nothing"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>